<commit_message>
Added alternate 5V LDO for U1.
</commit_message>
<xml_diff>
--- a/EE/v2.0/RCM-PBB_E1_BOM.xlsx
+++ b/EE/v2.0/RCM-PBB_E1_BOM.xlsx
@@ -1,25 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17030"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Donna\Desktop\Engineering3\Boards\RCM-PBB_E1\EE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Engineering-3\RCM-PBB_E1\EE\v2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADA988B-44D5-43E8-88F2-7D672BFA8204}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23700" windowHeight="8130"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23700" windowHeight="8130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RCM-PBB-E1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="178">
   <si>
     <t>Reference Designator</t>
   </si>
@@ -538,13 +546,28 @@
   </si>
   <si>
     <t>EN3-RCM-PBB-PCB+E1</t>
+  </si>
+  <si>
+    <t>L78L05ABUTR </t>
+  </si>
+  <si>
+    <t>Alt U1</t>
+  </si>
+  <si>
+    <t>497-1181-1-ND</t>
+  </si>
+  <si>
+    <t>IC REG LINEAR 5V 100MA SOT89-3</t>
+  </si>
+  <si>
+    <t>STMicroelectronics</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -580,6 +603,12 @@
       <b/>
       <sz val="8"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -623,7 +652,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -652,6 +681,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -990,11 +1020,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1110,13 +1140,13 @@
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="6">
-        <f t="shared" ref="I3:I31" si="0">10*F3</f>
+        <f t="shared" ref="I3:I32" si="0">10*F3</f>
         <v>20</v>
       </c>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6">
-        <f t="shared" ref="L3:L31" si="1">105*F3</f>
+        <f t="shared" ref="L3:L32" si="1">105*F3</f>
         <v>210</v>
       </c>
       <c r="M3" s="6"/>
@@ -1996,27 +2026,25 @@
       </c>
       <c r="M28" s="6"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" ht="12" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>24</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="B29" s="6"/>
       <c r="C29" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>48</v>
+        <v>177</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>173</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F29" s="7">
+        <v>175</v>
+      </c>
+      <c r="F29" s="10">
         <v>1</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>54</v>
+        <v>176</v>
       </c>
       <c r="H29" s="6"/>
       <c r="I29" s="6">
@@ -2033,118 +2061,153 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F30" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H30" s="6"/>
       <c r="I30" s="6">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
       <c r="L30" s="6">
         <f t="shared" si="1"/>
-        <v>210</v>
+        <v>105</v>
       </c>
       <c r="M30" s="6"/>
     </row>
-    <row r="31" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>108</v>
+        <v>26</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>136</v>
+        <v>52</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="F31" s="10">
-        <v>1</v>
+        <v>50</v>
+      </c>
+      <c r="F31" s="7">
+        <v>2</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>137</v>
+        <v>53</v>
       </c>
       <c r="H31" s="6"/>
       <c r="I31" s="6">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
       <c r="L31" s="6">
         <f t="shared" si="1"/>
-        <v>105</v>
+        <v>210</v>
       </c>
       <c r="M31" s="6"/>
     </row>
     <row r="32" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="B32" s="6"/>
+        <v>23</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>108</v>
+      </c>
       <c r="C32" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="F32" s="7">
+        <v>107</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F32" s="10">
         <v>1</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>172</v>
+        <v>137</v>
       </c>
       <c r="H32" s="6"/>
       <c r="I32" s="6">
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="J32" s="6"/>
       <c r="K32" s="6"/>
       <c r="L32" s="6">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
+      <c r="M32" s="6"/>
+    </row>
+    <row r="33" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="F33" s="7">
+        <v>1</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6">
+        <v>8</v>
+      </c>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6">
         <v>100</v>
       </c>
-      <c r="M32" s="6"/>
+      <c r="M33" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D23" r:id="rId1" display="http://www.digikey.com/product-detail/en/MCR10ERTF1912/RHM19.1KCHCT-ND/4084644"/>
-    <hyperlink ref="D22" r:id="rId2" display="http://www.digikey.com/product-detail/en/MCR10ERTF4992/RHM49.9KCHCT-ND/4084880"/>
-    <hyperlink ref="D24" r:id="rId3" display="http://www.digikey.com/product-detail/en/MCR10ERTF9311/RHM9.31KCHCT-ND/4085036"/>
-    <hyperlink ref="D21" r:id="rId4" display="http://www.digikey.com/product-detail/en/MCR10ERTF1002/RHM10.0KCHCT-ND/2796513"/>
-    <hyperlink ref="D16" r:id="rId5" display="http://www.digikey.com/product-detail/en/MCR10ERTF7500/RHM750CHCT-ND/4084981"/>
-    <hyperlink ref="D17" r:id="rId6" display="http://www.digikey.com/product-detail/en/MCR10ERTF1001/RHM1.00KCHCT-ND/2796512"/>
-    <hyperlink ref="D18" r:id="rId7" display="http://www.digikey.com/product-detail/en/MCR10ERTF2400/RHM240CHCT-ND/4084696"/>
-    <hyperlink ref="D19" r:id="rId8" display="http://www.digikey.com/product-detail/en/MCR10ERTF7153/RHM715KCHCT-ND/4084974"/>
-    <hyperlink ref="D20" r:id="rId9" display="http://www.digikey.com/product-detail/en/MCR10ERTF6193/RHM619KCHCT-ND/4084934"/>
-    <hyperlink ref="D25" r:id="rId10" display="http://www.digikey.com/product-detail/en/MCR10ERTF1052/RHM10.5KCHCT-ND/4084480"/>
-    <hyperlink ref="D15" r:id="rId11" display="http://www.digikey.com/product-detail/en/MCR10ERTF1000/RHM100CHCT-ND/2796511"/>
+    <hyperlink ref="D23" r:id="rId1" display="http://www.digikey.com/product-detail/en/MCR10ERTF1912/RHM19.1KCHCT-ND/4084644" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D22" r:id="rId2" display="http://www.digikey.com/product-detail/en/MCR10ERTF4992/RHM49.9KCHCT-ND/4084880" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D24" r:id="rId3" display="http://www.digikey.com/product-detail/en/MCR10ERTF9311/RHM9.31KCHCT-ND/4085036" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D21" r:id="rId4" display="http://www.digikey.com/product-detail/en/MCR10ERTF1002/RHM10.0KCHCT-ND/2796513" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D16" r:id="rId5" display="http://www.digikey.com/product-detail/en/MCR10ERTF7500/RHM750CHCT-ND/4084981" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D17" r:id="rId6" display="http://www.digikey.com/product-detail/en/MCR10ERTF1001/RHM1.00KCHCT-ND/2796512" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D18" r:id="rId7" display="http://www.digikey.com/product-detail/en/MCR10ERTF2400/RHM240CHCT-ND/4084696" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="D19" r:id="rId8" display="http://www.digikey.com/product-detail/en/MCR10ERTF7153/RHM715KCHCT-ND/4084974" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="D20" r:id="rId9" display="http://www.digikey.com/product-detail/en/MCR10ERTF6193/RHM619KCHCT-ND/4084934" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="D25" r:id="rId10" display="http://www.digikey.com/product-detail/en/MCR10ERTF1052/RHM10.5KCHCT-ND/4084480" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D15" r:id="rId11" display="http://www.digikey.com/product-detail/en/MCR10ERTF1000/RHM100CHCT-ND/2796511" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.25" header="0" footer="0"/>

</xml_diff>